<commit_message>
clean up figs & tables
</commit_message>
<xml_diff>
--- a/tables/supptable_S1.xlsx
+++ b/tables/supptable_S1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="294">
   <si>
     <t>Reference</t>
   </si>
@@ -860,9 +860,6 @@
     <t>Studies which use models to simulate/compare the impacts of different control and surveillance measures</t>
   </si>
   <si>
-    <t>Studies which use models to examine potential drivers of dynamics (separate category from explain observed patterns because sometimes do not use data or observations but use models as hypotheticals)</t>
-  </si>
-  <si>
     <t>Studies that use models to predict incidence and/or burden of rabies in the future given current estimates and data</t>
   </si>
   <si>
@@ -902,14 +899,20 @@
     <t>Next-generation matrix model to estimate transmission parameters; transmission tree reconstruction</t>
   </si>
   <si>
-    <t xml:space="preserve">Lloyd-Smith, et al. 2009 </t>
+    <t>[@lloyd-smithEpidemicDynamicsHumanAnimal2009]</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Studies which use models to examine potential drivers of dynamics (separate category from explain observed patterns because  do these do not use data or observations but use models as hypotheticals)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -964,6 +967,13 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -982,7 +992,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1166,8 +1176,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1205,11 +1225,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="193">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1301,6 +1322,11 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1392,6 +1418,11 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1949,7 +1980,7 @@
         <v>219</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="60" hidden="1">
@@ -2015,7 +2046,7 @@
         <v>212</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="45">
@@ -2274,7 +2305,7 @@
         <v>237</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="90">
@@ -2535,7 +2566,7 @@
         <v>243</v>
       </c>
       <c r="V12" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="75">
@@ -2808,7 +2839,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>114</v>
@@ -2859,7 +2890,7 @@
         <v>225</v>
       </c>
       <c r="V17" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="75" hidden="1">
@@ -3258,7 +3289,7 @@
         <v>241</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="45">
@@ -4101,7 +4132,7 @@
         <v>234</v>
       </c>
       <c r="V36" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="45" hidden="1">
@@ -4486,7 +4517,7 @@
         <v>220</v>
       </c>
       <c r="V42" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="60" hidden="1">
@@ -4878,7 +4909,7 @@
         <v>235</v>
       </c>
       <c r="V48" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="60" hidden="1">
@@ -5135,7 +5166,7 @@
         <v>250</v>
       </c>
       <c r="V52" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="53" spans="1:22">
@@ -5166,14 +5197,14 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="560" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="107.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="15" customFormat="1">
@@ -5194,6 +5225,9 @@
       <c r="B2" s="3" t="s">
         <v>267</v>
       </c>
+      <c r="C2" s="18" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
@@ -5202,6 +5236,9 @@
       <c r="B3" s="3" t="s">
         <v>270</v>
       </c>
+      <c r="C3" s="18" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
@@ -5210,6 +5247,9 @@
       <c r="B4" s="3" t="s">
         <v>271</v>
       </c>
+      <c r="C4" s="18" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
@@ -5218,6 +5258,9 @@
       <c r="B5" s="3" t="s">
         <v>272</v>
       </c>
+      <c r="C5" s="18" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
@@ -5226,6 +5269,9 @@
       <c r="B6" s="3" t="s">
         <v>273</v>
       </c>
+      <c r="C6" s="18" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
@@ -5234,6 +5280,9 @@
       <c r="B7" s="3" t="s">
         <v>274</v>
       </c>
+      <c r="C7" s="18" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1">
       <c r="A8" t="s">
@@ -5243,7 +5292,7 @@
         <v>275</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
@@ -5254,7 +5303,7 @@
         <v>276</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5265,24 +5314,26 @@
         <v>277</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C11" s="17"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" s="17" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>292</v>
@@ -5293,7 +5344,10 @@
         <v>201</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5301,7 +5355,10 @@
         <v>156</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -5309,7 +5366,10 @@
         <v>200</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30">
@@ -5317,63 +5377,87 @@
         <v>202</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>282</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>203</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>283</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>204</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>284</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>205</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>285</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>151</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>286</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>159</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>287</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>268</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>178</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -5393,7 +5477,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="560" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>